<commit_message>
Inclusao do driver chrome para webdriver
</commit_message>
<xml_diff>
--- a/sceweb/WebContent/WEB-INF/lib/roteiros_de_teste.xlsx
+++ b/sceweb/WebContent/WEB-INF/lib/roteiros_de_teste.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esa\git\scewebv2\sceweb\WebContent\WEB-INF\lib\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>cadastro realizado com sucesso</t>
   </si>
@@ -27,24 +32,9 @@
     <t>89424232000180</t>
   </si>
   <si>
-    <t>21/04/2017</t>
-  </si>
-  <si>
-    <t>21/04/2018</t>
-  </si>
-  <si>
-    <t>80195205000109</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>erro - cadastro nao realizado</t>
-  </si>
-  <si>
-    <t>formConvenio</t>
-  </si>
-  <si>
     <t>acao</t>
   </si>
   <si>
@@ -57,9 +47,6 @@
     <t>estado de chegada</t>
   </si>
   <si>
-    <t>cadastrarConvenio</t>
-  </si>
-  <si>
     <t>formEmpresa</t>
   </si>
   <si>
@@ -120,19 +107,13 @@
     <t>coluna13</t>
   </si>
   <si>
-    <t>excluirConvenio</t>
-  </si>
-  <si>
     <t>excluirEmpresa</t>
-  </si>
-  <si>
-    <t>abreFormConvenio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,14 +152,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -486,269 +466,161 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1"/>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>